<commit_message>
+1 neptuniana Database v0.04
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mis Cosas\Mis Proyectos\Solar War\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A24E25-56AE-4623-A9DC-E3537AF33028}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7864C7EE-4BCC-406B-B815-AA116FAD330B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
   <si>
     <t>CARTA</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Cuesta 1  de M.O. menos por cada punto de vida que le falte al 'Corazón de crisálida'</t>
+  </si>
+  <si>
+    <t>Devota de La Crisálida</t>
+  </si>
+  <si>
+    <t>Cuando muere, busca en el mazo una carta de M.O. y ponla en juego. Baraja el mazo.</t>
   </si>
 </sst>
 </file>
@@ -550,7 +556,7 @@
   <dimension ref="A1:O551"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,15 +887,31 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2</v>
+      </c>
+      <c r="F13" s="5">
+        <v>3</v>
+      </c>
+      <c r="G13" s="5">
+        <v>2</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>

</xml_diff>

<commit_message>
Database v0.07 + Pulido
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\Solar-War\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mis Cosas\Mis Proyectos\Solar War\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FF5148-ECDE-4923-B892-A6EEB449842F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E3979A-8319-4125-8760-4128CD61FD12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="52">
   <si>
     <t>CARTA</t>
   </si>
@@ -173,6 +173,15 @@
   <si>
     <t>Cuando una criatura ataque al nucleo, gana el control de la criatura permanentemente</t>
   </si>
+  <si>
+    <t>Cría de Insecto Ópalo</t>
+  </si>
+  <si>
+    <t>Poco común</t>
+  </si>
+  <si>
+    <t>Tras morir restaura 3 puntos de vida al 'Corazón crisálida'</t>
+  </si>
 </sst>
 </file>
 
@@ -264,7 +273,41 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -314,6 +357,40 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
   </dxfs>
@@ -601,7 +678,7 @@
   <dimension ref="A1:O555"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,14 +1192,30 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
+      <c r="A20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="5">
+        <v>2</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -6392,15 +6485,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"Común"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Poco común"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Mauina de Guerra, DDBB v.0.08
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\Solar-War\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FF5148-ECDE-4923-B892-A6EEB449842F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D96BCCE-9286-4F7E-83EF-E95CAF73C9BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="50">
   <si>
     <t>CARTA</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Comandante</t>
   </si>
   <si>
-    <t xml:space="preserve"> +1 / +1 por cada soldado en juego</t>
-  </si>
-  <si>
     <t>Mina Explosiva</t>
   </si>
   <si>
@@ -172,6 +169,12 @@
   </si>
   <si>
     <t>Cuando una criatura ataque al nucleo, gana el control de la criatura permanentemente</t>
+  </si>
+  <si>
+    <t>Maquina de guerra</t>
+  </si>
+  <si>
+    <t>Entra en CB en PA cuando muere regresa en PD con 3/5</t>
   </si>
 </sst>
 </file>
@@ -598,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O555"/>
+  <dimension ref="A1:O556"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,39 +859,39 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>15</v>
+      <c r="E10" s="3">
+        <v>5</v>
+      </c>
+      <c r="F10" s="5">
+        <v>3</v>
       </c>
       <c r="G10" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>7</v>
@@ -900,73 +903,73 @@
         <v>15</v>
       </c>
       <c r="G11" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="3">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5">
-        <v>1</v>
+      <c r="E12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="G12" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>15</v>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1</v>
       </c>
       <c r="G13" s="5">
-        <v>0</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>28</v>
+        <v>5</v>
+      </c>
+      <c r="H13" s="5">
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>7</v>
@@ -974,25 +977,25 @@
       <c r="E14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="5">
-        <v>20</v>
-      </c>
-      <c r="G14" s="3" t="s">
+      <c r="F14" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="G14" s="5">
+        <v>0</v>
+      </c>
       <c r="H14" s="5" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>7</v>
@@ -1000,45 +1003,45 @@
       <c r="E15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>15</v>
+      <c r="F15" s="5">
+        <v>20</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="3">
-        <v>8</v>
-      </c>
-      <c r="F16" s="5">
-        <v>8</v>
-      </c>
-      <c r="G16" s="5">
+      <c r="E16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="9" t="s">
-        <v>31</v>
+      <c r="F16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>17</v>
@@ -1050,53 +1053,53 @@
         <v>7</v>
       </c>
       <c r="E17" s="3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F17" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G17" s="5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>15</v>
+      <c r="E18" s="3">
+        <v>2</v>
+      </c>
+      <c r="F18" s="5">
+        <v>3</v>
       </c>
       <c r="G18" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>7</v>
@@ -1107,22 +1110,38 @@
       <c r="F19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="5">
+        <v>3</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="F20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -2824,12 +2843,12 @@
       <c r="G190" s="5"/>
       <c r="H190" s="5"/>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A191" s="5"/>
-      <c r="B191" s="5"/>
-      <c r="C191" s="5"/>
-      <c r="D191" s="5"/>
-      <c r="E191" s="5"/>
+    <row r="191" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A191" s="3"/>
+      <c r="B191" s="3"/>
+      <c r="C191" s="3"/>
+      <c r="D191" s="3"/>
+      <c r="E191" s="3"/>
       <c r="F191" s="5"/>
       <c r="G191" s="5"/>
       <c r="H191" s="5"/>
@@ -5635,9 +5654,10 @@
       <c r="H471" s="5"/>
     </row>
     <row r="472" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A472" s="6"/>
-      <c r="B472" s="6"/>
-      <c r="D472" s="6"/>
+      <c r="A472" s="5"/>
+      <c r="B472" s="5"/>
+      <c r="C472" s="5"/>
+      <c r="D472" s="5"/>
       <c r="E472" s="5"/>
       <c r="F472" s="5"/>
       <c r="G472" s="5"/>
@@ -6389,6 +6409,15 @@
       <c r="F555" s="5"/>
       <c r="G555" s="5"/>
       <c r="H555" s="5"/>
+    </row>
+    <row r="556" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A556" s="6"/>
+      <c r="B556" s="6"/>
+      <c r="D556" s="6"/>
+      <c r="E556" s="5"/>
+      <c r="F556" s="5"/>
+      <c r="G556" s="5"/>
+      <c r="H556" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">

</xml_diff>

<commit_message>
Soldado Elite DDBB v0.10
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\Solar-War\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB21267-E326-413C-A57B-5CECCE9E8777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C63E3B1-CA2E-4C42-9F4B-B0015AE05940}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="58">
   <si>
     <t>CARTA</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>Invoca a 1 1/1 por 1 de maná</t>
+  </si>
+  <si>
+    <t>Soldado de Élite</t>
+  </si>
+  <si>
+    <t>Sigilo, Impacto Crítico</t>
   </si>
 </sst>
 </file>
@@ -636,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O557"/>
+  <dimension ref="A1:O558"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,9 +872,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
@@ -880,53 +886,53 @@
         <v>7</v>
       </c>
       <c r="E9" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F9" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G9" s="5">
         <v>6</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H9" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>15</v>
+      <c r="E10" s="3">
+        <v>5</v>
+      </c>
+      <c r="F10" s="5">
+        <v>3</v>
       </c>
       <c r="G10" s="5">
-        <v>3</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>7</v>
@@ -940,13 +946,13 @@
       <c r="G11" s="5">
         <v>3</v>
       </c>
-      <c r="H11" s="9" t="s">
-        <v>47</v>
+      <c r="H11" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
@@ -964,67 +970,67 @@
         <v>15</v>
       </c>
       <c r="G12" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="3">
-        <v>1</v>
-      </c>
-      <c r="F13" s="5">
-        <v>1</v>
+      <c r="E13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="G13" s="5">
-        <v>5</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>43</v>
+        <v>6</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>15</v>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1</v>
       </c>
       <c r="G14" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>4</v>
@@ -1042,21 +1048,21 @@
         <v>15</v>
       </c>
       <c r="G15" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>7</v>
@@ -1064,25 +1070,25 @@
       <c r="E16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="5">
-        <v>20</v>
-      </c>
-      <c r="G16" s="3" t="s">
+      <c r="F16" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="G16" s="5">
+        <v>0</v>
+      </c>
       <c r="H16" s="5" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>7</v>
@@ -1090,45 +1096,45 @@
       <c r="E17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>15</v>
+      <c r="F17" s="5">
+        <v>20</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="3">
-        <v>8</v>
-      </c>
-      <c r="F18" s="5">
-        <v>8</v>
-      </c>
-      <c r="G18" s="5">
+      <c r="E18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="9" t="s">
-        <v>31</v>
+      <c r="F18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>17</v>
@@ -1140,53 +1146,53 @@
         <v>7</v>
       </c>
       <c r="E19" s="3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F19" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G19" s="5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>15</v>
+      <c r="E20" s="3">
+        <v>2</v>
+      </c>
+      <c r="F20" s="5">
+        <v>3</v>
       </c>
       <c r="G20" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>7</v>
@@ -1197,48 +1203,64 @@
       <c r="F21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="3" t="s">
-        <v>15</v>
+      <c r="G21" s="5">
+        <v>3</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E23" s="3">
         <v>1</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F23" s="5">
         <v>2</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G23" s="5">
         <v>1</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
@@ -2930,12 +2952,12 @@
       <c r="G192" s="5"/>
       <c r="H192" s="5"/>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A193" s="5"/>
-      <c r="B193" s="5"/>
-      <c r="C193" s="5"/>
-      <c r="D193" s="5"/>
-      <c r="E193" s="5"/>
+    <row r="193" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A193" s="3"/>
+      <c r="B193" s="3"/>
+      <c r="C193" s="3"/>
+      <c r="D193" s="3"/>
+      <c r="E193" s="3"/>
       <c r="F193" s="5"/>
       <c r="G193" s="5"/>
       <c r="H193" s="5"/>
@@ -5741,9 +5763,10 @@
       <c r="H473" s="5"/>
     </row>
     <row r="474" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A474" s="6"/>
-      <c r="B474" s="6"/>
-      <c r="D474" s="6"/>
+      <c r="A474" s="5"/>
+      <c r="B474" s="5"/>
+      <c r="C474" s="5"/>
+      <c r="D474" s="5"/>
       <c r="E474" s="5"/>
       <c r="F474" s="5"/>
       <c r="G474" s="5"/>
@@ -6495,6 +6518,15 @@
       <c r="F557" s="5"/>
       <c r="G557" s="5"/>
       <c r="H557" s="5"/>
+    </row>
+    <row r="558" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A558" s="6"/>
+      <c r="B558" s="6"/>
+      <c r="D558" s="6"/>
+      <c r="E558" s="5"/>
+      <c r="F558" s="5"/>
+      <c r="G558" s="5"/>
+      <c r="H558" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">

</xml_diff>

<commit_message>
Munición Incendiaria DDBB v0.12
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\Solar-War\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7A96BD-5213-429C-8A87-6AAE04F2D4CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D30F544-9D97-4100-AF84-2FE5D030D61B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="60">
   <si>
     <t>CARTA</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Sigilo, Impacto Crítico</t>
+  </si>
+  <si>
+    <t>Municion Incendiaria</t>
+  </si>
+  <si>
+    <t>da +2/+0 a los aliados</t>
   </si>
 </sst>
 </file>
@@ -642,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O558"/>
+  <dimension ref="A1:O559"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,7 +932,7 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
@@ -946,19 +952,19 @@
       <c r="G11" s="5">
         <v>3</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="H11" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>7</v>
@@ -972,13 +978,13 @@
       <c r="G12" s="5">
         <v>3</v>
       </c>
-      <c r="H12" s="9" t="s">
-        <v>47</v>
+      <c r="H12" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>4</v>
@@ -996,67 +1002,67 @@
         <v>15</v>
       </c>
       <c r="G13" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="3">
-        <v>1</v>
-      </c>
-      <c r="F14" s="5">
-        <v>1</v>
+      <c r="E14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="G14" s="5">
-        <v>5</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>43</v>
+        <v>6</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>15</v>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5">
+        <v>1</v>
       </c>
       <c r="G15" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>4</v>
@@ -1074,21 +1080,21 @@
         <v>15</v>
       </c>
       <c r="G16" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>7</v>
@@ -1096,25 +1102,25 @@
       <c r="E17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="5">
-        <v>20</v>
-      </c>
-      <c r="G17" s="3" t="s">
+      <c r="F17" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="G17" s="5">
+        <v>0</v>
+      </c>
       <c r="H17" s="5" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>7</v>
@@ -1122,45 +1128,45 @@
       <c r="E18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>15</v>
+      <c r="F18" s="5">
+        <v>20</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="3">
-        <v>8</v>
-      </c>
-      <c r="F19" s="5">
-        <v>8</v>
-      </c>
-      <c r="G19" s="5">
+      <c r="E19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>31</v>
+      <c r="F19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>17</v>
@@ -1172,53 +1178,53 @@
         <v>7</v>
       </c>
       <c r="E20" s="3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F20" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G20" s="5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>15</v>
+      <c r="E21" s="3">
+        <v>2</v>
+      </c>
+      <c r="F21" s="5">
+        <v>3</v>
       </c>
       <c r="G21" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>7</v>
@@ -1229,48 +1235,64 @@
       <c r="F22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>15</v>
+      <c r="G22" s="5">
+        <v>3</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E24" s="3">
         <v>1</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F24" s="5">
         <v>2</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G24" s="5">
         <v>1</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -2962,12 +2984,12 @@
       <c r="G193" s="5"/>
       <c r="H193" s="5"/>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A194" s="5"/>
-      <c r="B194" s="5"/>
-      <c r="C194" s="5"/>
-      <c r="D194" s="5"/>
-      <c r="E194" s="5"/>
+    <row r="194" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A194" s="3"/>
+      <c r="B194" s="3"/>
+      <c r="C194" s="3"/>
+      <c r="D194" s="3"/>
+      <c r="E194" s="3"/>
       <c r="F194" s="5"/>
       <c r="G194" s="5"/>
       <c r="H194" s="5"/>
@@ -5773,9 +5795,10 @@
       <c r="H474" s="5"/>
     </row>
     <row r="475" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A475" s="6"/>
-      <c r="B475" s="6"/>
-      <c r="D475" s="6"/>
+      <c r="A475" s="5"/>
+      <c r="B475" s="5"/>
+      <c r="C475" s="5"/>
+      <c r="D475" s="5"/>
       <c r="E475" s="5"/>
       <c r="F475" s="5"/>
       <c r="G475" s="5"/>
@@ -6527,6 +6550,15 @@
       <c r="F558" s="5"/>
       <c r="G558" s="5"/>
       <c r="H558" s="5"/>
+    </row>
+    <row r="559" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A559" s="6"/>
+      <c r="B559" s="6"/>
+      <c r="D559" s="6"/>
+      <c r="E559" s="5"/>
+      <c r="F559" s="5"/>
+      <c r="G559" s="5"/>
+      <c r="H559" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">

</xml_diff>

<commit_message>
Database v 0.16 + (leer desc)
+ Huevo palpitante
* Cuerno protector
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\Solar-War\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mis Cosas\Mis Proyectos\Solar War\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EF137B-9451-4BFC-9E04-D54243566B11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556314BE-BA79-406F-8B4D-F3700CC2978E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="68">
   <si>
     <t>CARTA</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Equipo</t>
   </si>
   <si>
-    <t>Otorga escudo permanente y +1/+0 este turno a un esbirro aliado</t>
-  </si>
-  <si>
     <t>Escudo</t>
   </si>
   <si>
@@ -217,6 +214,21 @@
   </si>
   <si>
     <t>Criatura no puede ser objetivo de habilidades hasta que ataque</t>
+  </si>
+  <si>
+    <t>Explosión de M.O.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inflinge 2 puntos de daño a todos los esbirros y héroes enemigos </t>
+  </si>
+  <si>
+    <t>Huevo palpitante</t>
+  </si>
+  <si>
+    <t>Otorga escudo y +1/+0 este turno a los esbirros adyacentes.</t>
+  </si>
+  <si>
+    <t>Al morir regresa como una araña 3/3</t>
   </si>
 </sst>
 </file>
@@ -663,7 +675,7 @@
   <dimension ref="A1:O560"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,7 +904,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
@@ -913,12 +925,12 @@
         <v>6</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
@@ -939,12 +951,12 @@
         <v>6</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
@@ -965,12 +977,12 @@
         <v>3</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
@@ -991,18 +1003,18 @@
         <v>3</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>7</v>
@@ -1017,18 +1029,18 @@
         <v>3</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>7</v>
@@ -1043,12 +1055,12 @@
         <v>6</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>4</v>
@@ -1069,12 +1081,12 @@
         <v>5</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>4</v>
@@ -1095,12 +1107,12 @@
         <v>2</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>4</v>
@@ -1121,7 +1133,7 @@
         <v>2</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1254,7 +1266,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>34</v>
       </c>
@@ -1265,7 +1277,7 @@
         <v>35</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>15</v>
@@ -1277,18 +1289,18 @@
         <v>3</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>7</v>
@@ -1303,12 +1315,12 @@
         <v>15</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>17</v>
@@ -1317,7 +1329,7 @@
         <v>8</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E25" s="3">
         <v>1</v>
@@ -1329,12 +1341,12 @@
         <v>1</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>17</v>
@@ -1355,28 +1367,60 @@
         <v>5</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="5">
+        <v>4</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
+      <c r="A28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>2</v>
+      </c>
+      <c r="G28" s="5">
+        <v>2</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>

</xml_diff>

<commit_message>
+ 3 cartas neptunianos y DDBB v0.19
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\Solar-War\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mis Cosas\Mis Proyectos\Solar War\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5E16D1-E37B-41DE-8A4F-673B5962A342}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8FC5B4-94BB-40CF-94AE-9BE2ECAE1249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="78">
   <si>
     <t>CARTA</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Monstruo Mecánico</t>
   </si>
   <si>
-    <t>Si hay mecánico en juego suma contador +0/+1</t>
-  </si>
-  <si>
     <t>Daña primero</t>
   </si>
   <si>
@@ -235,13 +232,74 @@
   </si>
   <si>
     <t>Al dañar a 1 criatura daña en 1 pto al héroe o núcleo objetivo.</t>
+  </si>
+  <si>
+    <t>Cefalópodo estelar</t>
+  </si>
+  <si>
+    <t>Gana +0/+1 al ser invocada por cada carta en la mano del jugador. (No se tienen en cuenta las cartas de maná)</t>
+  </si>
+  <si>
+    <t>Prestidigitación</t>
+  </si>
+  <si>
+    <t>Blast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inflinge 1 de daño a una criatura y roba una carta. </t>
+  </si>
+  <si>
+    <t>Gigante de mediodía</t>
+  </si>
+  <si>
+    <t>Cuesta 1  de M.O. menos por cada carta en la mano del jugador.</t>
+  </si>
+  <si>
+    <r>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Si hay mecánico en juego suma </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>contador</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> +0/+1</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,6 +318,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -327,7 +392,75 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -681,7 +814,7 @@
   <dimension ref="A1:O561"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,8 +930,8 @@
       <c r="F4" s="3">
         <v>2</v>
       </c>
-      <c r="G4" s="5">
-        <v>4</v>
+      <c r="G4" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>21</v>
@@ -879,7 +1012,7 @@
         <v>3</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -905,12 +1038,12 @@
         <v>4</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
@@ -931,12 +1064,12 @@
         <v>6</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
@@ -957,12 +1090,12 @@
         <v>5</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
@@ -983,12 +1116,12 @@
         <v>6</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
@@ -1009,12 +1142,12 @@
         <v>3</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>4</v>
@@ -1035,18 +1168,18 @@
         <v>3</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>7</v>
@@ -1061,18 +1194,18 @@
         <v>3</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>7</v>
@@ -1087,12 +1220,12 @@
         <v>6</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>4</v>
@@ -1113,18 +1246,18 @@
         <v>5</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>7</v>
@@ -1139,18 +1272,18 @@
         <v>2</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>7</v>
@@ -1165,18 +1298,18 @@
         <v>2</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>7</v>
@@ -1191,7 +1324,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1222,7 +1355,7 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>17</v>
@@ -1248,7 +1381,7 @@
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>17</v>
@@ -1269,12 +1402,12 @@
         <v>15</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>17</v>
@@ -1295,21 +1428,21 @@
         <v>2</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>15</v>
@@ -1321,18 +1454,18 @@
         <v>3</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>7</v>
@@ -1347,12 +1480,12 @@
         <v>15</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>17</v>
@@ -1361,7 +1494,7 @@
         <v>8</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E26" s="3">
         <v>1</v>
@@ -1373,12 +1506,12 @@
         <v>1</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>17</v>
@@ -1399,12 +1532,12 @@
         <v>5</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>17</v>
@@ -1425,12 +1558,12 @@
         <v>4</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>17</v>
@@ -1451,38 +1584,86 @@
         <v>2</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="3">
+        <v>2</v>
+      </c>
+      <c r="F30" s="5">
+        <v>1</v>
+      </c>
+      <c r="G30" s="5">
+        <v>3</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
+      <c r="A31" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="5">
+        <v>2</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="3">
+        <v>8</v>
+      </c>
+      <c r="F32" s="5">
+        <v>8</v>
+      </c>
+      <c r="G32" s="5">
+        <v>12</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
@@ -6691,19 +6872,35 @@
       <c r="H561" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="D1:D31 D33:D1048576">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>"Poco común"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+      <formula>"Común"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B31 B33:B1048576">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>"Neptunianos"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>"Federación de comercio"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="B32">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
+2 poderes de núcleo neptuniano DDBB v0.19
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mis Cosas\Mis Proyectos\Solar War\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8FC5B4-94BB-40CF-94AE-9BE2ECAE1249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F743C8-B19D-42BB-971B-887AF58111E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="82">
   <si>
     <t>CARTA</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Torreta de defensa</t>
-  </si>
-  <si>
-    <t>Poder de nucleo</t>
   </si>
   <si>
     <t>Hace 1 pto de daño a la criatura o jugador objetivo</t>
@@ -293,6 +290,21 @@
       </rPr>
       <t xml:space="preserve"> +0/+1</t>
     </r>
+  </si>
+  <si>
+    <t>Sacrificio premeditado</t>
+  </si>
+  <si>
+    <t>Poder de núcleo</t>
+  </si>
+  <si>
+    <t>Coste de utilización: 2 Recibe 2 puntos de daño y roba una cara</t>
+  </si>
+  <si>
+    <t>Absorción de vida</t>
+  </si>
+  <si>
+    <t>Coste de utilización: 2. Inflinge 2 ptos de daño y restaura 2 ptos de salud al 'Corazón Crisálida'</t>
   </si>
 </sst>
 </file>
@@ -392,7 +404,143 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -813,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O561"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,7 +1079,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>21</v>
@@ -1012,7 +1160,7 @@
         <v>3</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1043,7 +1191,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
@@ -1064,12 +1212,12 @@
         <v>6</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
@@ -1090,12 +1238,12 @@
         <v>5</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
@@ -1116,12 +1264,12 @@
         <v>6</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
@@ -1142,12 +1290,12 @@
         <v>3</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>4</v>
@@ -1168,18 +1316,18 @@
         <v>3</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>7</v>
@@ -1194,18 +1342,18 @@
         <v>3</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>7</v>
@@ -1220,12 +1368,12 @@
         <v>6</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>4</v>
@@ -1246,18 +1394,18 @@
         <v>5</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>7</v>
@@ -1272,18 +1420,18 @@
         <v>2</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>7</v>
@@ -1298,7 +1446,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1309,7 +1457,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>7</v>
@@ -1324,7 +1472,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1355,7 +1503,7 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>17</v>
@@ -1381,7 +1529,7 @@
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>17</v>
@@ -1402,12 +1550,12 @@
         <v>15</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>17</v>
@@ -1428,21 +1576,21 @@
         <v>2</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>15</v>
@@ -1454,18 +1602,18 @@
         <v>3</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>7</v>
@@ -1480,12 +1628,12 @@
         <v>15</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>17</v>
@@ -1494,7 +1642,7 @@
         <v>8</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="3">
         <v>1</v>
@@ -1506,12 +1654,12 @@
         <v>1</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>17</v>
@@ -1532,12 +1680,12 @@
         <v>5</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>17</v>
@@ -1558,12 +1706,12 @@
         <v>4</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>17</v>
@@ -1584,12 +1732,12 @@
         <v>2</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>17</v>
@@ -1610,18 +1758,18 @@
         <v>3</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>7</v>
@@ -1636,12 +1784,12 @@
         <v>2</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>17</v>
@@ -1662,28 +1810,60 @@
         <v>12</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
+      <c r="A33" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="5">
+        <v>0</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="5">
+        <v>3</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
@@ -6872,36 +7052,68 @@
       <c r="H561" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D31 D33:D1048576">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+  <conditionalFormatting sqref="D1:D31 D35:D1048576">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B31 B33:B1048576">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+  <conditionalFormatting sqref="B1:B31 B35:B1048576">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>"Federación de comercio"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"Neptunianos"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"Federación de comercio"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"Poco común"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"Común"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Neptunianos"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"Federación de comercio"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Poco común"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ingeniero de combate + SistemaDefensaCompleto
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\Solar-War\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5E16D1-E37B-41DE-8A4F-673B5962A342}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B6CABC-AD08-4260-82CE-FD4272F14564}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,9 +201,6 @@
     <t>Municion Incendiaria</t>
   </si>
   <si>
-    <t>da +2/+0 a los aliados</t>
-  </si>
-  <si>
     <t>Insecto Ópalo</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t>Al dañar a 1 criatura daña en 1 pto al héroe o núcleo objetivo.</t>
+  </si>
+  <si>
+    <t>da +2/+0 a los aliados hasta final turno</t>
   </si>
 </sst>
 </file>
@@ -681,7 +681,7 @@
   <dimension ref="A1:O561"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,7 +936,7 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
@@ -957,7 +957,7 @@
         <v>5</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -1009,7 +1009,7 @@
         <v>3</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1118,7 +1118,7 @@
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>4</v>
@@ -1139,7 +1139,7 @@
         <v>2</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1321,7 +1321,7 @@
         <v>3</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1378,7 +1378,7 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>17</v>
@@ -1399,12 +1399,12 @@
         <v>5</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>17</v>
@@ -1425,12 +1425,12 @@
         <v>4</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>17</v>
@@ -1451,7 +1451,7 @@
         <v>2</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
+2 cartas NEP + Rareza Épico DDBB v0.21
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\Solar-War\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mis Cosas\Mis Proyectos\Solar War\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38ABE8A4-4E04-4E25-8F3F-E13A4CF2C43D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612EF37A-4D50-475F-BD63-1F1A95AD3105}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="93">
   <si>
     <t>CARTA</t>
   </si>
@@ -317,6 +317,27 @@
   </si>
   <si>
     <t>Duplica daño torreta de defensa y afecta a todos los enemigos</t>
+  </si>
+  <si>
+    <t>Controlador de masas</t>
+  </si>
+  <si>
+    <t>Al ser invocado, si el oponente controla más de 3 criaturas, toma el control de una al azar.</t>
+  </si>
+  <si>
+    <t>Golpe de sangre</t>
+  </si>
+  <si>
+    <t>Destruye la criatura o héroe objetivo. Recibe 3 puntos de daño</t>
+  </si>
+  <si>
+    <t>Exiliado</t>
+  </si>
+  <si>
+    <t>Épico</t>
+  </si>
+  <si>
+    <t>Al ser invocado, pone en juego una criatura aleatoria del oponente</t>
   </si>
 </sst>
 </file>
@@ -416,28 +437,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="55">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FFCC00FF"/>
         </patternFill>
       </fill>
       <border>
@@ -556,7 +560,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
       <border>
@@ -573,7 +577,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF9966FF"/>
+          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
       <border>
@@ -689,10 +693,691 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC00FF"/>
       <color rgb="FF9966FF"/>
       <color rgb="FF6600FF"/>
     </mruColors>
@@ -973,8 +1658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O563"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,35 +2614,83 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" s="3">
+        <v>3</v>
+      </c>
+      <c r="F37" s="5">
+        <v>3</v>
+      </c>
+      <c r="G37" s="5">
+        <v>4</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
+      <c r="A38" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="5">
+        <v>6</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E39" s="3">
+        <v>3</v>
+      </c>
+      <c r="F39" s="5">
+        <v>5</v>
+      </c>
+      <c r="G39" s="5">
+        <v>2</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
@@ -7116,68 +7849,113 @@
       <c r="H563" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D33 D37:D1048576">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+  <conditionalFormatting sqref="D1:D33 D39:D1048576">
+    <cfRule type="cellIs" dxfId="54" priority="26" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="31" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B33 B37:B1048576">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+  <conditionalFormatting sqref="B1:B33 B40:B1048576">
+    <cfRule type="cellIs" dxfId="52" priority="27" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="29" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="22" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="25" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="23" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="24" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="20" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="21" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="18" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="19" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="16" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="17" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="14" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="15" operator="equal">
       <formula>"Común"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37">
+    <cfRule type="cellIs" dxfId="38" priority="12" operator="equal">
+      <formula>"Neptunianos"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="13" operator="equal">
+      <formula>"Federación de comercio"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="cellIs" dxfId="36" priority="8" operator="equal">
+      <formula>"Poco común"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="9" operator="equal">
+      <formula>"Común"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
+      <formula>"Neptunianos"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
+      <formula>"Federación de comercio"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
+      <formula>"Poco común"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+      <formula>"Común"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+      <formula>"Neptunianos"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+      <formula>"Federación de comercio"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Épico"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
+Melontha Madre + DDBB v0.22
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mis Cosas\Mis Proyectos\Solar War\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612EF37A-4D50-475F-BD63-1F1A95AD3105}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AC9970-D239-486A-8340-38D2D0C5FAFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="95">
   <si>
     <t>CARTA</t>
   </si>
@@ -331,13 +331,19 @@
     <t>Destruye la criatura o héroe objetivo. Recibe 3 puntos de daño</t>
   </si>
   <si>
-    <t>Exiliado</t>
-  </si>
-  <si>
     <t>Épico</t>
   </si>
   <si>
     <t>Al ser invocado, pone en juego una criatura aleatoria del oponente</t>
+  </si>
+  <si>
+    <t>Exiliado de plutón</t>
+  </si>
+  <si>
+    <t>Melontha madre</t>
+  </si>
+  <si>
+    <t>Al morir, invoca una cría melontha 1/2 con escudo</t>
   </si>
 </sst>
 </file>
@@ -437,58 +443,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC00FF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9966FF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="31">
     <dxf>
       <fill>
         <patternFill>
@@ -560,364 +515,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9966FF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9966FF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9966FF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9966FF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9966FF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FFCC00FF"/>
         </patternFill>
       </fill>
       <border>
@@ -1658,8 +1256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O563"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2668,7 +2266,7 @@
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>17</v>
@@ -2677,7 +2275,7 @@
         <v>8</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E39" s="3">
         <v>3</v>
@@ -2689,18 +2287,34 @@
         <v>2</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
+      <c r="A40" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E40" s="3">
+        <v>3</v>
+      </c>
+      <c r="F40" s="5">
+        <v>5</v>
+      </c>
+      <c r="G40" s="5">
+        <v>5</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
@@ -7850,112 +7464,128 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D33 D39:D1048576">
-    <cfRule type="cellIs" dxfId="54" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B33 B40:B1048576">
-    <cfRule type="cellIs" dxfId="52" priority="27" operator="equal">
+  <conditionalFormatting sqref="B1:B33 B41:B1048576">
+    <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="cellIs" dxfId="50" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="cellIs" dxfId="48" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="28" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="cellIs" dxfId="46" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="44" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="cellIs" dxfId="42" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="40" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="cellIs" dxfId="38" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="cellIs" dxfId="36" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Épico"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Neptunianos"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"Federación de comercio"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Poco común"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
+2 cards. rareza Legendario. DDBB v0.24
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\Solar-War\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mis Cosas\Mis Proyectos\Solar War\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93433FFC-6DFB-4239-9302-A25F91D6B8F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C521F62F-CA36-44B2-A071-2D652426BB84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="117">
   <si>
     <t>CARTA</t>
   </si>
@@ -378,12 +378,91 @@
   <si>
     <t>1- Roba 1 carta.    2- Cambia la posicion de combate de la criatura objetivo.    3- Destruye la carta maná objetivo. Daña todos los núcleos en 2 ptos. Invoca un soldado droide 2/1.</t>
   </si>
+  <si>
+    <t>El Vidente</t>
+  </si>
+  <si>
+    <t>Restaura 3 'Contenedor de M.O.' Adivina 2 cartas. Roba 1.</t>
+  </si>
+  <si>
+    <t>Legendario</t>
+  </si>
+  <si>
+    <t>Anulador de energías</t>
+  </si>
+  <si>
+    <t>Anula la próxima habilidad enemiga</t>
+  </si>
+  <si>
+    <t>La bestia</t>
+  </si>
+  <si>
+    <t>Anaconda</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pasiva - El </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Corazón Crisálida'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es invulnerable. 1 - (-1) Gana 3 de vida al inicio de tu próximo turno. Pasiva - al recibir daño invoca una cría melontha 1/2 con escudo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Golpe </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- (-1) Inflinge 2 de daño a una criatura o héroe. 2 - (Gratis) Se convierte en una criatura con ataque y vida igual al número de veces que se usó golpe.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Yolanda </t>
+  </si>
+  <si>
+    <t>Invulnerable. 1-(-1) Adivina una carta 2-(-2) Busca una carta de maná en tu mazo y colócala en el campo de batalla. 3-(-3)Devuelve una carta del cementerio a la mano</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,6 +488,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -476,11 +563,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="87">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
+          <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
       <border>
@@ -497,7 +584,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FF9966FF"/>
         </patternFill>
       </fill>
       <border>
@@ -548,7 +635,959 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFCC00FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966FF"/>
         </patternFill>
       </fill>
       <border>
@@ -1289,8 +2328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O568"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2480,54 +3519,134 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
+      <c r="A46" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E46" s="3">
+        <v>4</v>
+      </c>
+      <c r="F46" s="5">
+        <v>4</v>
+      </c>
+      <c r="G46" s="5">
+        <v>7</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-    </row>
-    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-    </row>
-    <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-    </row>
-    <row r="50" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
+      <c r="A47" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G47" s="5">
+        <v>3</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="5">
+        <v>6</v>
+      </c>
+      <c r="G48" s="5">
+        <v>4</v>
+      </c>
+      <c r="H48" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="5">
+        <v>5</v>
+      </c>
+      <c r="G49" s="5">
+        <v>10</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" s="5">
+        <v>4</v>
+      </c>
+      <c r="G50" s="5">
+        <v>3</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
@@ -7627,115 +8746,198 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D38 D44:D1048576">
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="51" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="56" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B38 B46:B1048576">
-    <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
+  <conditionalFormatting sqref="B1:B38 B51:B1048576">
+    <cfRule type="cellIs" dxfId="84" priority="52" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="54" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39">
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="47" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="50" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="48" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="49" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="45" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="46" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="43" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="44" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="41" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="42" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41">
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="39" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="40" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="37" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="38" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="33" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="34" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="31" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="32" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="29" operator="equal">
       <formula>"Poco común"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="30" operator="equal">
       <formula>"Común"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="27" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="28" operator="equal">
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
       <formula>"Épico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+      <formula>"Legendario"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
+    <cfRule type="cellIs" dxfId="60" priority="24" operator="equal">
+      <formula>"Neptunianos"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="25" operator="equal">
+      <formula>"Federación de comercio"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule type="cellIs" dxfId="58" priority="22" operator="equal">
+      <formula>"Poco común"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="23" operator="equal">
+      <formula>"Común"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46">
+    <cfRule type="cellIs" dxfId="56" priority="20" operator="equal">
+      <formula>"Neptunianos"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="21" operator="equal">
+      <formula>"Federación de comercio"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46">
+    <cfRule type="cellIs" dxfId="54" priority="18" operator="equal">
+      <formula>"Poco común"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="19" operator="equal">
+      <formula>"Común"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+      <formula>"Neptunianos"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>"Federación de comercio"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+      <formula>"Poco común"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+      <formula>"Común"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>"Neptunianos"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"Federación de comercio"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"Poco común"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"Común"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48:D49">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"Poco común"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"Común"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"Poco común"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"Común"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Neptunianos"</formula>
     </cfRule>
@@ -7743,12 +8945,12 @@
       <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
+  <conditionalFormatting sqref="B50">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"Poco común"</formula>
+      <formula>"Neptunianos"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"Común"</formula>
+      <formula>"Federación de comercio"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>